<commit_message>
Update Leave Card 1/11/2024 4:44 pm
</commit_message>
<xml_diff>
--- a/CASUAL/LA PICNIC GROVE/ACUB, MA. MARILYN LANTING.xlsx
+++ b/CASUAL/LA PICNIC GROVE/ACUB, MA. MARILYN LANTING.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="139">
   <si>
     <t>PERIOD</t>
   </si>
@@ -435,6 +435,24 @@
   </si>
   <si>
     <t>UT(0-1-21)</t>
+  </si>
+  <si>
+    <t>UT(0-2-50)</t>
+  </si>
+  <si>
+    <t>UT(0-2-59)</t>
+  </si>
+  <si>
+    <t>UT(0-2-44)</t>
+  </si>
+  <si>
+    <t>UT(0-4 -59)</t>
+  </si>
+  <si>
+    <t>UT(0-0-59)</t>
+  </si>
+  <si>
+    <t>UT(0-1-32)</t>
   </si>
 </sst>
 </file>
@@ -1742,9 +1760,9 @@
   <dimension ref="A2:M130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A52" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A58" activePane="bottomLeft"/>
       <selection activeCell="F9" sqref="F9"/>
-      <selection pane="bottomLeft" activeCell="F75" sqref="F75"/>
+      <selection pane="bottomLeft" activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +1924,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])</f>
-        <v>58.991</v>
+        <v>56.983999999999995</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3045,11 +3063,15 @@
       <c r="A65" s="41">
         <v>44621</v>
       </c>
-      <c r="B65" s="20"/>
+      <c r="B65" s="20" t="s">
+        <v>138</v>
+      </c>
       <c r="C65" s="13">
         <v>1.25</v>
       </c>
-      <c r="D65" s="40"/>
+      <c r="D65" s="40">
+        <v>0.192</v>
+      </c>
       <c r="E65" s="9"/>
       <c r="F65" s="20"/>
       <c r="G65" s="13">
@@ -3065,11 +3087,15 @@
       <c r="A66" s="41">
         <v>44652</v>
       </c>
-      <c r="B66" s="20"/>
+      <c r="B66" s="20" t="s">
+        <v>137</v>
+      </c>
       <c r="C66" s="13">
         <v>1.25</v>
       </c>
-      <c r="D66" s="40"/>
+      <c r="D66" s="40">
+        <v>0.12300000000000001</v>
+      </c>
       <c r="E66" s="9"/>
       <c r="F66" s="20"/>
       <c r="G66" s="13">
@@ -3105,11 +3131,15 @@
       <c r="A68" s="41">
         <v>44713</v>
       </c>
-      <c r="B68" s="20"/>
+      <c r="B68" s="20" t="s">
+        <v>136</v>
+      </c>
       <c r="C68" s="13">
         <v>1.25</v>
       </c>
-      <c r="D68" s="40"/>
+      <c r="D68" s="40">
+        <v>0.623</v>
+      </c>
       <c r="E68" s="9"/>
       <c r="F68" s="20"/>
       <c r="G68" s="13">
@@ -3125,11 +3155,15 @@
       <c r="A69" s="41">
         <v>44743</v>
       </c>
-      <c r="B69" s="20"/>
+      <c r="B69" s="20" t="s">
+        <v>135</v>
+      </c>
       <c r="C69" s="13">
         <v>1.25</v>
       </c>
-      <c r="D69" s="40"/>
+      <c r="D69" s="40">
+        <v>0.34199999999999997</v>
+      </c>
       <c r="E69" s="9"/>
       <c r="F69" s="20"/>
       <c r="G69" s="13">
@@ -3145,11 +3179,15 @@
       <c r="A70" s="41">
         <v>44774</v>
       </c>
-      <c r="B70" s="20"/>
+      <c r="B70" s="20" t="s">
+        <v>134</v>
+      </c>
       <c r="C70" s="13">
         <v>1.25</v>
       </c>
-      <c r="D70" s="40"/>
+      <c r="D70" s="40">
+        <v>0.373</v>
+      </c>
       <c r="E70" s="9"/>
       <c r="F70" s="20"/>
       <c r="G70" s="13">
@@ -3165,11 +3203,15 @@
       <c r="A71" s="41">
         <v>44805</v>
       </c>
-      <c r="B71" s="20"/>
+      <c r="B71" s="20" t="s">
+        <v>133</v>
+      </c>
       <c r="C71" s="13">
         <v>1.25</v>
       </c>
-      <c r="D71" s="40"/>
+      <c r="D71" s="40">
+        <v>0.35399999999999998</v>
+      </c>
       <c r="E71" s="9"/>
       <c r="F71" s="20"/>
       <c r="G71" s="13">
@@ -6842,11 +6884,11 @@
         <v>1</v>
       </c>
       <c r="F3" s="11">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="G3" s="46">
         <f>SUM(D3,E4,F4)</f>
-        <v>0.16900000000000001</v>
+        <v>0.192</v>
       </c>
       <c r="J3" s="35"/>
       <c r="K3" s="36">
@@ -6865,7 +6907,7 @@
       </c>
       <c r="F4" s="1">
         <f>IF(F3=0,0,IF(ISBLANK(F3),"",VLOOKUP(F3,C7:D66,2)))</f>
-        <v>4.4000000000000004E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">

</xml_diff>